<commit_message>
Cargar usuarios desde csv
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,28 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,11 +19,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Nombre</t>
   </si>
   <si>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Juan Torres Pardo</t>
+  </si>
+  <si>
+    <t>Luis López Fernandez</t>
+  </si>
+  <si>
+    <t>Sensor temperatura</t>
+  </si>
+  <si>
+    <t>Sensor humedad</t>
+  </si>
+  <si>
+    <t>Ana García Pérez</t>
+  </si>
+  <si>
+    <t>Bomberos de Asturias</t>
+  </si>
+  <si>
+    <t>juantp@example.com</t>
+  </si>
+  <si>
+    <t>organizacion1@example.com</t>
+  </si>
+  <si>
+    <t>luisgf@example.com</t>
+  </si>
+  <si>
+    <t>organizacion2@example.com</t>
+  </si>
+  <si>
+    <t>anagp@example.com</t>
+  </si>
+  <si>
+    <t>bomberosast@example.com</t>
+  </si>
+  <si>
     <t>90500084Y</t>
   </si>
   <si>
@@ -44,64 +81,25 @@
     <t>09940449X</t>
   </si>
   <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>C/ Real Oviedo 2</t>
-  </si>
-  <si>
-    <t>Av. De la Constitución 8</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>López Fernando</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
-    <t>Correo electrónico</t>
-  </si>
-  <si>
-    <t>juan@example.com</t>
-  </si>
-  <si>
-    <t>luis@example.com</t>
-  </si>
-  <si>
-    <t>ana@example.com</t>
-  </si>
-  <si>
-    <t>Dirección postal</t>
+    <t>43º 22' N, 5º 50' O</t>
+  </si>
+  <si>
+    <t>22º 17' N, 8º 75' S</t>
+  </si>
+  <si>
+    <t>78964566P</t>
+  </si>
+  <si>
+    <t>12348952O</t>
+  </si>
+  <si>
+    <t>23548912Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,12 +138,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -165,7 +161,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -210,9 +206,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -245,9 +241,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -426,119 +422,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21916</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{BE1B39A9-467D-48DF-8B4D-5FB77DCCC4BA}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{7727CB8B-FFEC-4ED3-AD0D-C2B6D59FC3A9}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{50A29618-0536-42BC-9072-2D9EACD74C7C}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{A141725A-D0E9-4956-8C9F-752C951AD798}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{AB9AB5A9-72A6-4A66-B732-A6033FF761B7}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{6AE77D8E-7FE1-47AF-BF3E-E49C828D06D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>